<commit_message>
Updated Kinect & EV3.
</commit_message>
<xml_diff>
--- a/Kinect/Ablauf.xlsx
+++ b/Kinect/Ablauf.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Vorne</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Links</t>
   </si>
   <si>
-    <t>Laufend</t>
-  </si>
-  <si>
     <t>Ablauf:</t>
   </si>
   <si>
@@ -45,12 +42,6 @@
     <t xml:space="preserve">    "Bitte … vor Roboter platzieren" (TextToSpeech)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Wenn Distanz &gt; vorherigeDistanz + X</t>
-  </si>
-  <si>
-    <t>~ 3 sec.</t>
-  </si>
-  <si>
     <t>~ 1 min.</t>
   </si>
   <si>
@@ -60,9 +51,6 @@
     <t>stehend</t>
   </si>
   <si>
-    <t>laufend</t>
-  </si>
-  <si>
     <t>laufend/stehend</t>
   </si>
   <si>
@@ -78,18 +66,12 @@
     <t>Algorithmus</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>OpenCV: SURF</t>
   </si>
   <si>
     <t>Bilder machen nach "OK" + lernen</t>
   </si>
   <si>
-    <t>Bild machen sobald bewegt (s.o.)</t>
-  </si>
-  <si>
     <t>Bild mit 5 Referenzen (Bilder, s.o.)vergleichen + Position auslesen</t>
   </si>
   <si>
@@ -97,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">    Warten auf "OK" von Person (SpeechRecognizer) oder warten bis Person erkannt -&gt; Handy und Laptop unabhängig</t>
+  </si>
+  <si>
+    <t>Standard</t>
   </si>
 </sst>
 </file>
@@ -199,64 +184,6 @@
             <a:gd name="adj1" fmla="val 8333"/>
             <a:gd name="adj2" fmla="val 37090"/>
           </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>4753</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>10783</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>110660</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>186906</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Geschweifte Klammer rechts 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29FD8BA3-F620-48A2-9409-EA2E4D4D6F54}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2760923" y="1344283"/>
-          <a:ext cx="105907" cy="176123"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBrace">
-          <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
@@ -550,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G14"/>
+  <dimension ref="C3:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +493,7 @@
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -580,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
@@ -588,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -596,85 +523,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>18</v>
+      <c r="G11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>